<commit_message>
updates to climate stuff
</commit_message>
<xml_diff>
--- a/climate/noaa_estimates.xlsx
+++ b/climate/noaa_estimates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\MultiGrain\climate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1AFE9F-E7FD-4EC2-BD1A-6A9201C3713E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5801DB1-300D-4D7E-A4F5-3B5A7953E9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1008,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" topLeftCell="D28" workbookViewId="0">
+      <selection activeCell="R42" sqref="R42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1187,43 +1187,43 @@
         <v>37.083999999999996</v>
       </c>
       <c r="M15">
-        <f>B15*12</f>
+        <f t="shared" ref="M15:V15" si="0">B15*12</f>
         <v>99.364800000000002</v>
       </c>
       <c r="N15">
-        <f>C15*12</f>
+        <f t="shared" si="0"/>
         <v>128.62559999999999</v>
       </c>
       <c r="O15">
-        <f>D15*12</f>
+        <f t="shared" si="0"/>
         <v>171.60239999999999</v>
       </c>
       <c r="P15">
-        <f>E15*12</f>
+        <f t="shared" si="0"/>
         <v>204.52079999999998</v>
       </c>
       <c r="Q15">
-        <f>F15*12</f>
+        <f t="shared" si="0"/>
         <v>248.71679999999998</v>
       </c>
       <c r="R15">
-        <f>G15*12</f>
+        <f t="shared" si="0"/>
         <v>282.8544</v>
       </c>
       <c r="S15">
-        <f>H15*12</f>
+        <f t="shared" si="0"/>
         <v>320.03999999999996</v>
       </c>
       <c r="T15">
-        <f>I15*12</f>
+        <f t="shared" si="0"/>
         <v>356.61599999999999</v>
       </c>
       <c r="U15">
-        <f>J15*12</f>
+        <f t="shared" si="0"/>
         <v>405.38399999999996</v>
       </c>
       <c r="V15">
-        <f>K15*12</f>
+        <f t="shared" si="0"/>
         <v>445.00799999999992</v>
       </c>
     </row>
@@ -1262,43 +1262,43 @@
         <v>56.388000000000005</v>
       </c>
       <c r="M16">
-        <f>B16*6</f>
+        <f t="shared" ref="M16:V16" si="1">B16*6</f>
         <v>75.590400000000002</v>
       </c>
       <c r="N16">
-        <f>C16*6</f>
+        <f t="shared" si="1"/>
         <v>97.840800000000002</v>
       </c>
       <c r="O16">
-        <f>D16*6</f>
+        <f t="shared" si="1"/>
         <v>130.75919999999999</v>
       </c>
       <c r="P16">
-        <f>E16*6</f>
+        <f t="shared" si="1"/>
         <v>155.44799999999998</v>
       </c>
       <c r="Q16">
-        <f>F16*6</f>
+        <f t="shared" si="1"/>
         <v>188.976</v>
       </c>
       <c r="R16">
-        <f>G16*6</f>
+        <f t="shared" si="1"/>
         <v>214.88399999999996</v>
       </c>
       <c r="S16">
-        <f>H16*6</f>
+        <f t="shared" si="1"/>
         <v>242.31600000000003</v>
       </c>
       <c r="T16">
-        <f>I16*6</f>
+        <f t="shared" si="1"/>
         <v>271.27199999999999</v>
       </c>
       <c r="U16">
-        <f>J16*6</f>
+        <f t="shared" si="1"/>
         <v>307.84800000000001</v>
       </c>
       <c r="V16">
-        <f>K16*6</f>
+        <f t="shared" si="1"/>
         <v>338.32800000000003</v>
       </c>
     </row>
@@ -1337,43 +1337,43 @@
         <v>69.849999999999994</v>
       </c>
       <c r="M17">
-        <f>B17*4</f>
+        <f t="shared" ref="M17:V17" si="2">B17*4</f>
         <v>62.483999999999995</v>
       </c>
       <c r="N17">
-        <f>C17*4</f>
+        <f t="shared" si="2"/>
         <v>80.873599999999996</v>
       </c>
       <c r="O17">
-        <f>D17*4</f>
+        <f t="shared" si="2"/>
         <v>107.696</v>
       </c>
       <c r="P17">
-        <f>E17*4</f>
+        <f t="shared" si="2"/>
         <v>129.03199999999998</v>
       </c>
       <c r="Q17">
-        <f>F17*4</f>
+        <f t="shared" si="2"/>
         <v>156.464</v>
       </c>
       <c r="R17">
-        <f>G17*4</f>
+        <f t="shared" si="2"/>
         <v>177.79999999999998</v>
       </c>
       <c r="S17">
-        <f>H17*4</f>
+        <f t="shared" si="2"/>
         <v>200.15199999999999</v>
       </c>
       <c r="T17">
-        <f>I17*4</f>
+        <f t="shared" si="2"/>
         <v>223.52</v>
       </c>
       <c r="U17">
-        <f>J17*4</f>
+        <f t="shared" si="2"/>
         <v>255.01599999999996</v>
       </c>
       <c r="V17">
-        <f>K17*4</f>
+        <f t="shared" si="2"/>
         <v>279.39999999999998</v>
       </c>
     </row>
@@ -1412,43 +1412,43 @@
         <v>94.233999999999995</v>
       </c>
       <c r="M18">
-        <f>B18*2</f>
+        <f t="shared" ref="M18:V18" si="3">B18*2</f>
         <v>42.062399999999997</v>
       </c>
       <c r="N18">
-        <f>C18*2</f>
+        <f t="shared" si="3"/>
         <v>54.356000000000002</v>
       </c>
       <c r="O18">
-        <f>D18*2</f>
+        <f t="shared" si="3"/>
         <v>72.643999999999991</v>
       </c>
       <c r="P18">
-        <f>E18*2</f>
+        <f t="shared" si="3"/>
         <v>86.867999999999995</v>
       </c>
       <c r="Q18">
-        <f>F18*2</f>
+        <f t="shared" si="3"/>
         <v>105.15599999999999</v>
       </c>
       <c r="R18">
-        <f>G18*2</f>
+        <f t="shared" si="3"/>
         <v>119.88799999999999</v>
       </c>
       <c r="S18">
-        <f>H18*2</f>
+        <f t="shared" si="3"/>
         <v>135.12799999999999</v>
       </c>
       <c r="T18">
-        <f>I18*2</f>
+        <f t="shared" si="3"/>
         <v>150.36799999999999</v>
       </c>
       <c r="U18">
-        <f>J18*2</f>
+        <f t="shared" si="3"/>
         <v>171.70399999999998</v>
       </c>
       <c r="V18">
-        <f>K18*2</f>
+        <f t="shared" si="3"/>
         <v>188.46799999999999</v>
       </c>
     </row>
@@ -1487,43 +1487,43 @@
         <v>116.58599999999998</v>
       </c>
       <c r="M19">
-        <f>B19</f>
+        <f t="shared" ref="M19:V19" si="4">B19</f>
         <v>26.161999999999999</v>
       </c>
       <c r="N19">
-        <f>C19</f>
+        <f t="shared" si="4"/>
         <v>33.781999999999996</v>
       </c>
       <c r="O19">
-        <f>D19</f>
+        <f t="shared" si="4"/>
         <v>44.957999999999998</v>
       </c>
       <c r="P19">
-        <f>E19</f>
+        <f t="shared" si="4"/>
         <v>53.593999999999994</v>
       </c>
       <c r="Q19">
-        <f>F19</f>
+        <f t="shared" si="4"/>
         <v>65.024000000000001</v>
       </c>
       <c r="R19">
-        <f>G19</f>
+        <f t="shared" si="4"/>
         <v>74.167999999999992</v>
       </c>
       <c r="S19">
-        <f>H19</f>
+        <f t="shared" si="4"/>
         <v>83.566000000000003</v>
       </c>
       <c r="T19">
-        <f>I19</f>
+        <f t="shared" si="4"/>
         <v>93.217999999999989</v>
       </c>
       <c r="U19">
-        <f>J19</f>
+        <f t="shared" si="4"/>
         <v>106.17199999999998</v>
       </c>
       <c r="V19">
-        <f>K19</f>
+        <f t="shared" si="4"/>
         <v>116.58599999999998</v>
       </c>
     </row>
@@ -1562,43 +1562,43 @@
         <v>147.57399999999998</v>
       </c>
       <c r="M20">
-        <f>B20/2</f>
+        <f t="shared" ref="M20:V20" si="5">B20/2</f>
         <v>14.731999999999998</v>
       </c>
       <c r="N20">
-        <f>C20/2</f>
+        <f t="shared" si="5"/>
         <v>19.177</v>
       </c>
       <c r="O20">
-        <f>D20/2</f>
+        <f t="shared" si="5"/>
         <v>26.034999999999997</v>
       </c>
       <c r="P20">
-        <f>E20/2</f>
+        <f t="shared" si="5"/>
         <v>31.369</v>
       </c>
       <c r="Q20">
-        <f>F20/2</f>
+        <f t="shared" si="5"/>
         <v>38.734999999999992</v>
       </c>
       <c r="R20">
-        <f>G20/2</f>
+        <f t="shared" si="5"/>
         <v>44.576999999999998</v>
       </c>
       <c r="S20">
-        <f>H20/2</f>
+        <f t="shared" si="5"/>
         <v>50.8</v>
       </c>
       <c r="T20">
-        <f>I20/2</f>
+        <f t="shared" si="5"/>
         <v>57.403999999999989</v>
       </c>
       <c r="U20">
-        <f>J20/2</f>
+        <f t="shared" si="5"/>
         <v>66.421000000000006</v>
       </c>
       <c r="V20">
-        <f>K20/2</f>
+        <f t="shared" si="5"/>
         <v>73.786999999999992</v>
       </c>
     </row>
@@ -1637,43 +1637,43 @@
         <v>159.00399999999999</v>
       </c>
       <c r="M21">
-        <f>B21/3</f>
+        <f t="shared" ref="M21:V21" si="6">B21/3</f>
         <v>10.583333333333334</v>
       </c>
       <c r="N21">
-        <f>C21/3</f>
+        <f t="shared" si="6"/>
         <v>13.716000000000001</v>
       </c>
       <c r="O21">
-        <f>D21/3</f>
+        <f t="shared" si="6"/>
         <v>18.541999999999998</v>
       </c>
       <c r="P21">
-        <f>E21/3</f>
+        <f t="shared" si="6"/>
         <v>22.352</v>
       </c>
       <c r="Q21">
-        <f>F21/3</f>
+        <f t="shared" si="6"/>
         <v>27.601333333333329</v>
       </c>
       <c r="R21">
-        <f>G21/3</f>
+        <f t="shared" si="6"/>
         <v>31.834666666666664</v>
       </c>
       <c r="S21">
-        <f>H21/3</f>
+        <f t="shared" si="6"/>
         <v>36.321999999999996</v>
       </c>
       <c r="T21">
-        <f>I21/3</f>
+        <f t="shared" si="6"/>
         <v>41.063333333333325</v>
       </c>
       <c r="U21">
-        <f>J21/3</f>
+        <f t="shared" si="6"/>
         <v>47.582666666666661</v>
       </c>
       <c r="V21">
-        <f>K21/3</f>
+        <f t="shared" si="6"/>
         <v>53.001333333333328</v>
       </c>
     </row>
@@ -1712,43 +1712,43 @@
         <v>176.78399999999999</v>
       </c>
       <c r="M22">
-        <f>B22/6</f>
+        <f t="shared" ref="M22:V22" si="7">B22/6</f>
         <v>6.0536666666666656</v>
       </c>
       <c r="N22">
-        <f>C22/6</f>
+        <f t="shared" si="7"/>
         <v>7.7893333333333326</v>
       </c>
       <c r="O22">
-        <f>D22/6</f>
+        <f t="shared" si="7"/>
         <v>10.414</v>
       </c>
       <c r="P22">
-        <f>E22/6</f>
+        <f t="shared" si="7"/>
         <v>12.488333333333335</v>
       </c>
       <c r="Q22">
-        <f>F22/6</f>
+        <f t="shared" si="7"/>
         <v>15.409333333333334</v>
       </c>
       <c r="R22">
-        <f>G22/6</f>
+        <f t="shared" si="7"/>
         <v>17.737666666666666</v>
       </c>
       <c r="S22">
-        <f>H22/6</f>
+        <f t="shared" si="7"/>
         <v>20.235333333333333</v>
       </c>
       <c r="T22">
-        <f>I22/6</f>
+        <f t="shared" si="7"/>
         <v>22.86</v>
       </c>
       <c r="U22">
-        <f>J22/6</f>
+        <f t="shared" si="7"/>
         <v>26.500666666666664</v>
       </c>
       <c r="V22">
-        <f>K22/6</f>
+        <f t="shared" si="7"/>
         <v>29.463999999999999</v>
       </c>
     </row>
@@ -1787,43 +1787,43 @@
         <v>199.136</v>
       </c>
       <c r="M23">
-        <f>B23/12</f>
+        <f t="shared" ref="M23:V23" si="8">B23/12</f>
         <v>3.4713333333333325</v>
       </c>
       <c r="N23">
-        <f>C23/12</f>
+        <f t="shared" si="8"/>
         <v>4.4449999999999994</v>
       </c>
       <c r="O23">
-        <f>D23/12</f>
+        <f t="shared" si="8"/>
         <v>5.9055</v>
       </c>
       <c r="P23">
-        <f>E23/12</f>
+        <f t="shared" si="8"/>
         <v>7.0908333333333333</v>
       </c>
       <c r="Q23">
-        <f>F23/12</f>
+        <f t="shared" si="8"/>
         <v>8.7206666666666663</v>
       </c>
       <c r="R23">
-        <f>G23/12</f>
+        <f t="shared" si="8"/>
         <v>10.032999999999999</v>
       </c>
       <c r="S23">
-        <f>H23/12</f>
+        <f t="shared" si="8"/>
         <v>11.43</v>
       </c>
       <c r="T23">
-        <f>I23/12</f>
+        <f t="shared" si="8"/>
         <v>12.890499999999998</v>
       </c>
       <c r="U23">
-        <f>J23/12</f>
+        <f t="shared" si="8"/>
         <v>14.943666666666665</v>
       </c>
       <c r="V23">
-        <f>K23/12</f>
+        <f t="shared" si="8"/>
         <v>16.594666666666665</v>
       </c>
     </row>
@@ -1862,43 +1862,43 @@
         <v>213.10599999999999</v>
       </c>
       <c r="M24">
-        <f>B24/24</f>
+        <f t="shared" ref="M24:V24" si="9">B24/24</f>
         <v>1.9261666666666668</v>
       </c>
       <c r="N24">
-        <f>C24/24</f>
+        <f t="shared" si="9"/>
         <v>2.4870833333333331</v>
       </c>
       <c r="O24">
-        <f>D24/24</f>
+        <f t="shared" si="9"/>
         <v>3.2808333333333333</v>
       </c>
       <c r="P24">
-        <f>E24/24</f>
+        <f t="shared" si="9"/>
         <v>3.9158333333333335</v>
       </c>
       <c r="Q24">
-        <f>F24/24</f>
+        <f t="shared" si="9"/>
         <v>4.7942499999999999</v>
       </c>
       <c r="R24">
-        <f>G24/24</f>
+        <f t="shared" si="9"/>
         <v>5.4821666666666653</v>
       </c>
       <c r="S24">
-        <f>H24/24</f>
+        <f t="shared" si="9"/>
         <v>6.212416666666666</v>
       </c>
       <c r="T24">
-        <f>I24/24</f>
+        <f t="shared" si="9"/>
         <v>6.9744166666666665</v>
       </c>
       <c r="U24">
-        <f>J24/24</f>
+        <f t="shared" si="9"/>
         <v>8.0327499999999983</v>
       </c>
       <c r="V24">
-        <f>K24/24</f>
+        <f t="shared" si="9"/>
         <v>8.8794166666666658</v>
       </c>
     </row>
@@ -1937,43 +1937,43 @@
         <v>264.15999999999997</v>
       </c>
       <c r="M25">
-        <f>B25/48</f>
+        <f t="shared" ref="M25:V25" si="10">B25/48</f>
         <v>1.0900833333333333</v>
       </c>
       <c r="N25">
-        <f>C25/48</f>
+        <f t="shared" si="10"/>
         <v>1.4022916666666665</v>
       </c>
       <c r="O25">
-        <f>D25/48</f>
+        <f t="shared" si="10"/>
         <v>1.8679583333333332</v>
       </c>
       <c r="P25">
-        <f>E25/48</f>
+        <f t="shared" si="10"/>
         <v>2.2489583333333329</v>
       </c>
       <c r="Q25">
-        <f>F25/48</f>
+        <f t="shared" si="10"/>
         <v>2.7887083333333327</v>
       </c>
       <c r="R25">
-        <f>G25/48</f>
+        <f t="shared" si="10"/>
         <v>3.2279166666666659</v>
       </c>
       <c r="S25">
-        <f>H25/48</f>
+        <f t="shared" si="10"/>
         <v>3.6935833333333332</v>
       </c>
       <c r="T25">
-        <f>I25/48</f>
+        <f t="shared" si="10"/>
         <v>4.1962916666666663</v>
       </c>
       <c r="U25">
-        <f>J25/48</f>
+        <f t="shared" si="10"/>
         <v>4.9053749999999994</v>
       </c>
       <c r="V25">
-        <f>K25/48</f>
+        <f t="shared" si="10"/>
         <v>5.503333333333333</v>
       </c>
     </row>
@@ -2362,43 +2362,43 @@
         <v>42.417999999999999</v>
       </c>
       <c r="M37">
-        <f>B37*12</f>
+        <f t="shared" ref="M37:V37" si="11">B37*12</f>
         <v>113.99519999999998</v>
       </c>
       <c r="N37">
-        <f>C37*12</f>
+        <f t="shared" si="11"/>
         <v>147.82799999999997</v>
       </c>
       <c r="O37">
-        <f>D37*12</f>
+        <f t="shared" si="11"/>
         <v>196.596</v>
       </c>
       <c r="P37">
-        <f>E37*12</f>
+        <f t="shared" si="11"/>
         <v>233.7816</v>
       </c>
       <c r="Q37">
-        <f>F37*12</f>
+        <f t="shared" si="11"/>
         <v>283.7688</v>
       </c>
       <c r="R37">
-        <f>G37*12</f>
+        <f t="shared" si="11"/>
         <v>323.08799999999997</v>
       </c>
       <c r="S37">
-        <f>H37*12</f>
+        <f t="shared" si="11"/>
         <v>362.71199999999993</v>
       </c>
       <c r="T37">
-        <f>I37*12</f>
+        <f t="shared" si="11"/>
         <v>405.38399999999996</v>
       </c>
       <c r="U37">
-        <f>J37*12</f>
+        <f t="shared" si="11"/>
         <v>463.29599999999994</v>
       </c>
       <c r="V37">
-        <f>K37*12</f>
+        <f t="shared" si="11"/>
         <v>509.01599999999996</v>
       </c>
     </row>
@@ -2437,43 +2437,43 @@
         <v>64.515999999999991</v>
       </c>
       <c r="M38">
-        <f>B38*6</f>
+        <f t="shared" ref="M38:V38" si="12">B38*6</f>
         <v>86.867999999999995</v>
       </c>
       <c r="N38">
-        <f>C38*6</f>
+        <f t="shared" si="12"/>
         <v>112.47119999999998</v>
       </c>
       <c r="O38">
-        <f>D38*6</f>
+        <f t="shared" si="12"/>
         <v>149.65679999999998</v>
       </c>
       <c r="P38">
-        <f>E38*6</f>
+        <f t="shared" si="12"/>
         <v>178.30799999999999</v>
       </c>
       <c r="Q38">
-        <f>F38*6</f>
+        <f t="shared" si="12"/>
         <v>216.40799999999999</v>
       </c>
       <c r="R38">
-        <f>G38*6</f>
+        <f t="shared" si="12"/>
         <v>245.36399999999998</v>
       </c>
       <c r="S38">
-        <f>H38*6</f>
+        <f t="shared" si="12"/>
         <v>275.84399999999999</v>
       </c>
       <c r="T38">
-        <f>I38*6</f>
+        <f t="shared" si="12"/>
         <v>307.84800000000001</v>
       </c>
       <c r="U38">
-        <f>J38*6</f>
+        <f t="shared" si="12"/>
         <v>352.04399999999998</v>
       </c>
       <c r="V38">
-        <f>K38*6</f>
+        <f t="shared" si="12"/>
         <v>387.09599999999995</v>
       </c>
     </row>
@@ -2512,43 +2512,43 @@
         <v>79.756</v>
       </c>
       <c r="M39">
-        <f>B39*4</f>
+        <f t="shared" ref="M39:V39" si="13">B39*4</f>
         <v>71.729599999999991</v>
       </c>
       <c r="N39">
-        <f>C39*4</f>
+        <f t="shared" si="13"/>
         <v>92.862399999999994</v>
       </c>
       <c r="O39">
-        <f>D39*4</f>
+        <f t="shared" si="13"/>
         <v>123.95199999999998</v>
       </c>
       <c r="P39">
-        <f>E39*4</f>
+        <f t="shared" si="13"/>
         <v>147.32</v>
       </c>
       <c r="Q39">
-        <f>F39*4</f>
+        <f t="shared" si="13"/>
         <v>178.816</v>
       </c>
       <c r="R39">
-        <f>G39*4</f>
+        <f t="shared" si="13"/>
         <v>203.2</v>
       </c>
       <c r="S39">
-        <f>H39*4</f>
+        <f t="shared" si="13"/>
         <v>228.6</v>
       </c>
       <c r="T39">
-        <f>I39*4</f>
+        <f t="shared" si="13"/>
         <v>255.01599999999996</v>
       </c>
       <c r="U39">
-        <f>J39*4</f>
+        <f t="shared" si="13"/>
         <v>290.57599999999996</v>
       </c>
       <c r="V39">
-        <f>K39*4</f>
+        <f t="shared" si="13"/>
         <v>319.024</v>
       </c>
     </row>
@@ -2587,43 +2587,43 @@
         <v>107.696</v>
       </c>
       <c r="M40">
-        <f>B40*2</f>
+        <f t="shared" ref="M40:V40" si="14">B40*2</f>
         <v>48.26</v>
       </c>
       <c r="N40">
-        <f>C40*2</f>
+        <f t="shared" si="14"/>
         <v>62.483999999999995</v>
       </c>
       <c r="O40">
-        <f>D40*2</f>
+        <f t="shared" si="14"/>
         <v>83.311999999999983</v>
       </c>
       <c r="P40">
-        <f>E40*2</f>
+        <f t="shared" si="14"/>
         <v>99.059999999999988</v>
       </c>
       <c r="Q40">
-        <f>F40*2</f>
+        <f t="shared" si="14"/>
         <v>120.396</v>
       </c>
       <c r="R40">
-        <f>G40*2</f>
+        <f t="shared" si="14"/>
         <v>136.65199999999999</v>
       </c>
       <c r="S40">
-        <f>H40*2</f>
+        <f t="shared" si="14"/>
         <v>153.92399999999998</v>
       </c>
       <c r="T40">
-        <f>I40*2</f>
+        <f t="shared" si="14"/>
         <v>171.70399999999998</v>
       </c>
       <c r="U40">
-        <f>J40*2</f>
+        <f t="shared" si="14"/>
         <v>195.57999999999998</v>
       </c>
       <c r="V40">
-        <f>K40*2</f>
+        <f t="shared" si="14"/>
         <v>215.392</v>
       </c>
     </row>
@@ -2662,43 +2662,43 @@
         <v>133.096</v>
       </c>
       <c r="M41">
-        <f>B41</f>
+        <f t="shared" ref="M41:V41" si="15">B41</f>
         <v>29.971999999999998</v>
       </c>
       <c r="N41">
-        <f>C41</f>
+        <f t="shared" si="15"/>
         <v>38.607999999999997</v>
       </c>
       <c r="O41">
-        <f>D41</f>
+        <f t="shared" si="15"/>
         <v>51.561999999999991</v>
       </c>
       <c r="P41">
-        <f>E41</f>
+        <f t="shared" si="15"/>
         <v>61.213999999999999</v>
       </c>
       <c r="Q41">
-        <f>F41</f>
+        <f t="shared" si="15"/>
         <v>74.421999999999997</v>
       </c>
       <c r="R41">
-        <f>G41</f>
+        <f t="shared" si="15"/>
         <v>84.581999999999994</v>
       </c>
       <c r="S41">
-        <f>H41</f>
+        <f t="shared" si="15"/>
         <v>95.25</v>
       </c>
       <c r="T41">
-        <f>I41</f>
+        <f t="shared" si="15"/>
         <v>106.17199999999998</v>
       </c>
       <c r="U41">
-        <f>J41</f>
+        <f t="shared" si="15"/>
         <v>121.15799999999999</v>
       </c>
       <c r="V41">
-        <f>K41</f>
+        <f t="shared" si="15"/>
         <v>133.096</v>
       </c>
     </row>
@@ -2737,43 +2737,43 @@
         <v>167.13200000000001</v>
       </c>
       <c r="M42">
-        <f>B42/2</f>
+        <f t="shared" ref="M42:V42" si="16">B42/2</f>
         <v>16.890999999999998</v>
       </c>
       <c r="N42">
-        <f>C42/2</f>
+        <f t="shared" si="16"/>
         <v>21.971</v>
       </c>
       <c r="O42">
-        <f>D42/2</f>
+        <f t="shared" si="16"/>
         <v>29.717999999999996</v>
       </c>
       <c r="P42">
-        <f>E42/2</f>
+        <f t="shared" si="16"/>
         <v>35.686999999999998</v>
       </c>
       <c r="Q42">
-        <f>F42/2</f>
+        <f t="shared" si="16"/>
         <v>43.942</v>
       </c>
       <c r="R42">
-        <f>G42/2</f>
+        <f t="shared" si="16"/>
         <v>50.545999999999999</v>
       </c>
       <c r="S42">
-        <f>H42/2</f>
+        <f t="shared" si="16"/>
         <v>57.657999999999994</v>
       </c>
       <c r="T42">
-        <f>I42/2</f>
+        <f t="shared" si="16"/>
         <v>64.897000000000006</v>
       </c>
       <c r="U42">
-        <f>J42/2</f>
+        <f t="shared" si="16"/>
         <v>75.183999999999997</v>
       </c>
       <c r="V42">
-        <f>K42/2</f>
+        <f t="shared" si="16"/>
         <v>83.566000000000003</v>
       </c>
     </row>
@@ -2812,43 +2812,43 @@
         <v>179.578</v>
       </c>
       <c r="M43">
-        <f>B43/3</f>
+        <f t="shared" ref="M43:V43" si="17">B43/3</f>
         <v>12.107333333333331</v>
       </c>
       <c r="N43">
-        <f>C43/3</f>
+        <f t="shared" si="17"/>
         <v>15.663333333333334</v>
       </c>
       <c r="O43">
-        <f>D43/3</f>
+        <f t="shared" si="17"/>
         <v>21.082000000000001</v>
       </c>
       <c r="P43">
-        <f>E43/3</f>
+        <f t="shared" si="17"/>
         <v>25.315333333333331</v>
       </c>
       <c r="Q43">
-        <f>F43/3</f>
+        <f t="shared" si="17"/>
         <v>31.242000000000001</v>
       </c>
       <c r="R43">
-        <f>G43/3</f>
+        <f t="shared" si="17"/>
         <v>35.983333333333327</v>
       </c>
       <c r="S43">
-        <f>H43/3</f>
+        <f t="shared" si="17"/>
         <v>40.978666666666662</v>
       </c>
       <c r="T43">
-        <f>I43/3</f>
+        <f t="shared" si="17"/>
         <v>46.312666666666665</v>
       </c>
       <c r="U43">
-        <f>J43/3</f>
+        <f t="shared" si="17"/>
         <v>53.763333333333328</v>
       </c>
       <c r="V43">
-        <f>K43/3</f>
+        <f t="shared" si="17"/>
         <v>59.859333333333332</v>
       </c>
     </row>
@@ -2887,43 +2887,43 @@
         <v>198.88199999999998</v>
       </c>
       <c r="M44">
-        <f>B44/6</f>
+        <f t="shared" ref="M44:V44" si="18">B44/6</f>
         <v>6.9003333333333323</v>
       </c>
       <c r="N44">
-        <f>C44/6</f>
+        <f t="shared" si="18"/>
         <v>8.8899999999999988</v>
       </c>
       <c r="O44">
-        <f>D44/6</f>
+        <f t="shared" si="18"/>
         <v>11.811</v>
       </c>
       <c r="P44">
-        <f>E44/6</f>
+        <f t="shared" si="18"/>
         <v>14.097</v>
       </c>
       <c r="Q44">
-        <f>F44/6</f>
+        <f t="shared" si="18"/>
         <v>17.356666666666666</v>
       </c>
       <c r="R44">
-        <f>G44/6</f>
+        <f t="shared" si="18"/>
         <v>19.938999999999997</v>
       </c>
       <c r="S44">
-        <f>H44/6</f>
+        <f t="shared" si="18"/>
         <v>22.733000000000001</v>
       </c>
       <c r="T44">
-        <f>I44/6</f>
+        <f t="shared" si="18"/>
         <v>25.696333333333332</v>
       </c>
       <c r="U44">
-        <f>J44/6</f>
+        <f t="shared" si="18"/>
         <v>29.802666666666667</v>
       </c>
       <c r="V44">
-        <f>K44/6</f>
+        <f t="shared" si="18"/>
         <v>33.146999999999998</v>
       </c>
     </row>
@@ -2962,43 +2962,43 @@
         <v>225.55200000000002</v>
       </c>
       <c r="M45">
-        <f>B45/12</f>
+        <f t="shared" ref="M45:V45" si="19">B45/12</f>
         <v>3.9581666666666666</v>
       </c>
       <c r="N45">
-        <f>C45/12</f>
+        <f t="shared" si="19"/>
         <v>5.0799999999999992</v>
       </c>
       <c r="O45">
-        <f>D45/12</f>
+        <f t="shared" si="19"/>
         <v>6.7098333333333331</v>
       </c>
       <c r="P45">
-        <f>E45/12</f>
+        <f t="shared" si="19"/>
         <v>8.043333333333333</v>
       </c>
       <c r="Q45">
-        <f>F45/12</f>
+        <f t="shared" si="19"/>
         <v>9.8636666666666653</v>
       </c>
       <c r="R45">
-        <f>G45/12</f>
+        <f t="shared" si="19"/>
         <v>11.345333333333334</v>
       </c>
       <c r="S45">
-        <f>H45/12</f>
+        <f t="shared" si="19"/>
         <v>12.911666666666664</v>
       </c>
       <c r="T45">
-        <f>I45/12</f>
+        <f t="shared" si="19"/>
         <v>14.562666666666665</v>
       </c>
       <c r="U45">
-        <f>J45/12</f>
+        <f t="shared" si="19"/>
         <v>16.891000000000002</v>
       </c>
       <c r="V45">
-        <f>K45/12</f>
+        <f t="shared" si="19"/>
         <v>18.796000000000003</v>
       </c>
     </row>
@@ -3037,43 +3037,43 @@
         <v>240.792</v>
       </c>
       <c r="M46">
-        <f>B46/24</f>
+        <f t="shared" ref="M46:V46" si="20">B46/24</f>
         <v>2.1801666666666666</v>
       </c>
       <c r="N46">
-        <f>C46/24</f>
+        <f t="shared" si="20"/>
         <v>2.804583333333333</v>
       </c>
       <c r="O46">
-        <f>D46/24</f>
+        <f t="shared" si="20"/>
         <v>3.7041666666666662</v>
       </c>
       <c r="P46">
-        <f>E46/24</f>
+        <f t="shared" si="20"/>
         <v>4.4132499999999997</v>
       </c>
       <c r="Q46">
-        <f>F46/24</f>
+        <f t="shared" si="20"/>
         <v>5.386916666666667</v>
       </c>
       <c r="R46">
-        <f>G46/24</f>
+        <f t="shared" si="20"/>
         <v>6.1595000000000004</v>
       </c>
       <c r="S46">
-        <f>H46/24</f>
+        <f t="shared" si="20"/>
         <v>6.9849999999999994</v>
       </c>
       <c r="T46">
-        <f>I46/24</f>
+        <f t="shared" si="20"/>
         <v>7.8422499999999999</v>
       </c>
       <c r="U46">
-        <f>J46/24</f>
+        <f t="shared" si="20"/>
         <v>9.0487500000000001</v>
       </c>
       <c r="V46">
-        <f>K46/24</f>
+        <f t="shared" si="20"/>
         <v>10.032999999999999</v>
       </c>
     </row>
@@ -3112,43 +3112,43 @@
         <v>302.26</v>
       </c>
       <c r="M47">
-        <f>B47/48</f>
+        <f t="shared" ref="M47:V47" si="21">B47/48</f>
         <v>1.2435416666666665</v>
       </c>
       <c r="N47">
-        <f>C47/48</f>
+        <f t="shared" si="21"/>
         <v>1.5980833333333333</v>
       </c>
       <c r="O47">
-        <f>D47/48</f>
+        <f t="shared" si="21"/>
         <v>2.1325416666666666</v>
       </c>
       <c r="P47">
-        <f>E47/48</f>
+        <f t="shared" si="21"/>
         <v>2.5611666666666664</v>
       </c>
       <c r="Q47">
-        <f>F47/48</f>
+        <f t="shared" si="21"/>
         <v>3.1644166666666664</v>
       </c>
       <c r="R47">
-        <f>G47/48</f>
+        <f t="shared" si="21"/>
         <v>3.6618333333333335</v>
       </c>
       <c r="S47">
-        <f>H47/48</f>
+        <f t="shared" si="21"/>
         <v>4.1909999999999998</v>
       </c>
       <c r="T47">
-        <f>I47/48</f>
+        <f t="shared" si="21"/>
         <v>4.7730833333333331</v>
       </c>
       <c r="U47">
-        <f>J47/48</f>
+        <f t="shared" si="21"/>
         <v>5.609166666666666</v>
       </c>
       <c r="V47">
-        <f>K47/48</f>
+        <f t="shared" si="21"/>
         <v>6.2970833333333331</v>
       </c>
     </row>
@@ -3537,43 +3537,43 @@
         <v>31.241999999999997</v>
       </c>
       <c r="M59">
-        <f>B59*12</f>
+        <f t="shared" ref="M59:V59" si="22">B59*12</f>
         <v>86.867999999999995</v>
       </c>
       <c r="N59">
-        <f>C59*12</f>
+        <f t="shared" si="22"/>
         <v>112.47119999999998</v>
       </c>
       <c r="O59">
-        <f>D59*12</f>
+        <f t="shared" si="22"/>
         <v>149.65679999999998</v>
       </c>
       <c r="P59">
-        <f>E59*12</f>
+        <f t="shared" si="22"/>
         <v>177.69839999999996</v>
       </c>
       <c r="Q59">
-        <f>F59*12</f>
+        <f t="shared" si="22"/>
         <v>214.88399999999996</v>
       </c>
       <c r="R59">
-        <f>G59*12</f>
+        <f t="shared" si="22"/>
         <v>243.53519999999997</v>
       </c>
       <c r="S59">
-        <f>H59*12</f>
+        <f t="shared" si="22"/>
         <v>272.79599999999999</v>
       </c>
       <c r="T59">
-        <f>I59*12</f>
+        <f t="shared" si="22"/>
         <v>302.66639999999995</v>
       </c>
       <c r="U59">
-        <f>J59*12</f>
+        <f t="shared" si="22"/>
         <v>341.37599999999998</v>
       </c>
       <c r="V59">
-        <f>K59*12</f>
+        <f t="shared" si="22"/>
         <v>374.904</v>
       </c>
     </row>
@@ -3612,43 +3612,43 @@
         <v>47.497999999999998</v>
       </c>
       <c r="M60">
-        <f>B60*6</f>
+        <f t="shared" ref="M60:V60" si="23">B60*6</f>
         <v>66.141599999999997</v>
       </c>
       <c r="N60">
-        <f>C60*6</f>
+        <f t="shared" si="23"/>
         <v>85.496400000000008</v>
       </c>
       <c r="O60">
-        <f>D60*6</f>
+        <f t="shared" si="23"/>
         <v>113.84279999999998</v>
       </c>
       <c r="P60">
-        <f>E60*6</f>
+        <f t="shared" si="23"/>
         <v>135.3312</v>
       </c>
       <c r="Q60">
-        <f>F60*6</f>
+        <f t="shared" si="23"/>
         <v>163.06800000000001</v>
       </c>
       <c r="R60">
-        <f>G60*6</f>
+        <f t="shared" si="23"/>
         <v>185.92799999999997</v>
       </c>
       <c r="S60">
-        <f>H60*6</f>
+        <f t="shared" si="23"/>
         <v>207.26400000000001</v>
       </c>
       <c r="T60">
-        <f>I60*6</f>
+        <f t="shared" si="23"/>
         <v>230.124</v>
       </c>
       <c r="U60">
-        <f>J60*6</f>
+        <f t="shared" si="23"/>
         <v>260.60399999999998</v>
       </c>
       <c r="V60">
-        <f>K60*6</f>
+        <f t="shared" si="23"/>
         <v>284.988</v>
       </c>
     </row>
@@ -3687,43 +3687,43 @@
         <v>58.673999999999999</v>
       </c>
       <c r="M61">
-        <f>B61*4</f>
+        <f t="shared" ref="M61:V61" si="24">B61*4</f>
         <v>54.660800000000002</v>
       </c>
       <c r="N61">
-        <f>C61*4</f>
+        <f t="shared" si="24"/>
         <v>70.713599999999985</v>
       </c>
       <c r="O61">
-        <f>D61*4</f>
+        <f t="shared" si="24"/>
         <v>94.081599999999995</v>
       </c>
       <c r="P61">
-        <f>E61*4</f>
+        <f t="shared" si="24"/>
         <v>111.76</v>
       </c>
       <c r="Q61">
-        <f>F61*4</f>
+        <f t="shared" si="24"/>
         <v>135.12799999999999</v>
       </c>
       <c r="R61">
-        <f>G61*4</f>
+        <f t="shared" si="24"/>
         <v>153.416</v>
       </c>
       <c r="S61">
-        <f>H61*4</f>
+        <f t="shared" si="24"/>
         <v>171.70399999999998</v>
       </c>
       <c r="T61">
-        <f>I61*4</f>
+        <f t="shared" si="24"/>
         <v>189.99199999999999</v>
       </c>
       <c r="U61">
-        <f>J61*4</f>
+        <f t="shared" si="24"/>
         <v>215.392</v>
       </c>
       <c r="V61">
-        <f>K61*4</f>
+        <f t="shared" si="24"/>
         <v>234.696</v>
       </c>
     </row>
@@ -3762,43 +3762,43 @@
         <v>78.993999999999986</v>
       </c>
       <c r="M62">
-        <f>B62*2</f>
+        <f t="shared" ref="M62:V62" si="25">B62*2</f>
         <v>36.83</v>
       </c>
       <c r="N62">
-        <f>C62*2</f>
+        <f t="shared" si="25"/>
         <v>47.599600000000002</v>
       </c>
       <c r="O62">
-        <f>D62*2</f>
+        <f t="shared" si="25"/>
         <v>63.5</v>
       </c>
       <c r="P62">
-        <f>E62*2</f>
+        <f t="shared" si="25"/>
         <v>75.183999999999997</v>
       </c>
       <c r="Q62">
-        <f>F62*2</f>
+        <f t="shared" si="25"/>
         <v>90.932000000000002</v>
       </c>
       <c r="R62">
-        <f>G62*2</f>
+        <f t="shared" si="25"/>
         <v>103.12399999999998</v>
       </c>
       <c r="S62">
-        <f>H62*2</f>
+        <f t="shared" si="25"/>
         <v>115.82399999999998</v>
       </c>
       <c r="T62">
-        <f>I62*2</f>
+        <f t="shared" si="25"/>
         <v>128.01599999999999</v>
       </c>
       <c r="U62">
-        <f>J62*2</f>
+        <f t="shared" si="25"/>
         <v>145.28799999999998</v>
       </c>
       <c r="V62">
-        <f>K62*2</f>
+        <f t="shared" si="25"/>
         <v>157.98799999999997</v>
       </c>
     </row>
@@ -3837,43 +3837,43 @@
         <v>97.789999999999992</v>
       </c>
       <c r="M63">
-        <f>B63</f>
+        <f t="shared" ref="M63:V63" si="26">B63</f>
         <v>22.783799999999999</v>
       </c>
       <c r="N63">
-        <f>C63</f>
+        <f t="shared" si="26"/>
         <v>29.463999999999995</v>
       </c>
       <c r="O63">
-        <f>D63</f>
+        <f t="shared" si="26"/>
         <v>39.116</v>
       </c>
       <c r="P63">
-        <f>E63</f>
+        <f t="shared" si="26"/>
         <v>46.481999999999999</v>
       </c>
       <c r="Q63">
-        <f>F63</f>
+        <f t="shared" si="26"/>
         <v>56.388000000000005</v>
       </c>
       <c r="R63">
-        <f>G63</f>
+        <f t="shared" si="26"/>
         <v>63.753999999999991</v>
       </c>
       <c r="S63">
-        <f>H63</f>
+        <f t="shared" si="26"/>
         <v>71.627999999999986</v>
       </c>
       <c r="T63">
-        <f>I63</f>
+        <f t="shared" si="26"/>
         <v>79.248000000000005</v>
       </c>
       <c r="U63">
-        <f>J63</f>
+        <f t="shared" si="26"/>
         <v>89.661999999999992</v>
       </c>
       <c r="V63">
-        <f>K63</f>
+        <f t="shared" si="26"/>
         <v>97.789999999999992</v>
       </c>
     </row>
@@ -3912,43 +3912,43 @@
         <v>123.18999999999998</v>
       </c>
       <c r="M64">
-        <f>B64/2</f>
+        <f t="shared" ref="M64:V64" si="27">B64/2</f>
         <v>12.953999999999999</v>
       </c>
       <c r="N64">
-        <f>C64/2</f>
+        <f t="shared" si="27"/>
         <v>16.763999999999999</v>
       </c>
       <c r="O64">
-        <f>D64/2</f>
+        <f t="shared" si="27"/>
         <v>22.733000000000001</v>
       </c>
       <c r="P64">
-        <f>E64/2</f>
+        <f t="shared" si="27"/>
         <v>27.304999999999996</v>
       </c>
       <c r="Q64">
-        <f>F64/2</f>
+        <f t="shared" si="27"/>
         <v>33.527999999999999</v>
       </c>
       <c r="R64">
-        <f>G64/2</f>
+        <f t="shared" si="27"/>
         <v>38.353999999999999</v>
       </c>
       <c r="S64">
-        <f>H64/2</f>
+        <f t="shared" si="27"/>
         <v>43.561</v>
       </c>
       <c r="T64">
-        <f>I64/2</f>
+        <f t="shared" si="27"/>
         <v>48.767999999999994</v>
       </c>
       <c r="U64">
-        <f>J64/2</f>
+        <f t="shared" si="27"/>
         <v>55.88</v>
       </c>
       <c r="V64">
-        <f>K64/2</f>
+        <f t="shared" si="27"/>
         <v>61.594999999999992</v>
       </c>
     </row>
@@ -3987,43 +3987,43 @@
         <v>132.07999999999998</v>
       </c>
       <c r="M65">
-        <f>B65/3</f>
+        <f t="shared" ref="M65:V65" si="28">B65/3</f>
         <v>9.3133333333333344</v>
       </c>
       <c r="N65">
-        <f>C65/3</f>
+        <f t="shared" si="28"/>
         <v>12.022666666666666</v>
       </c>
       <c r="O65">
-        <f>D65/3</f>
+        <f t="shared" si="28"/>
         <v>16.171333333333333</v>
       </c>
       <c r="P65">
-        <f>E65/3</f>
+        <f t="shared" si="28"/>
         <v>19.473333333333333</v>
       </c>
       <c r="Q65">
-        <f>F65/3</f>
+        <f t="shared" si="28"/>
         <v>23.875999999999994</v>
       </c>
       <c r="R65">
-        <f>G65/3</f>
+        <f t="shared" si="28"/>
         <v>27.432000000000002</v>
       </c>
       <c r="S65">
-        <f>H65/3</f>
+        <f t="shared" si="28"/>
         <v>31.072666666666663</v>
       </c>
       <c r="T65">
-        <f>I65/3</f>
+        <f t="shared" si="28"/>
         <v>34.798000000000002</v>
       </c>
       <c r="U65">
-        <f>J65/3</f>
+        <f t="shared" si="28"/>
         <v>39.962666666666664</v>
       </c>
       <c r="V65">
-        <f>K65/3</f>
+        <f t="shared" si="28"/>
         <v>44.026666666666664</v>
       </c>
     </row>
@@ -4062,43 +4062,43 @@
         <v>147.828</v>
       </c>
       <c r="M66">
-        <f>B66/6</f>
+        <f t="shared" ref="M66:V66" si="29">B66/6</f>
         <v>5.3339999999999996</v>
       </c>
       <c r="N66">
-        <f>C66/6</f>
+        <f t="shared" si="29"/>
         <v>6.9003333333333323</v>
       </c>
       <c r="O66">
-        <f>D66/6</f>
+        <f t="shared" si="29"/>
         <v>9.1440000000000001</v>
       </c>
       <c r="P66">
-        <f>E66/6</f>
+        <f t="shared" si="29"/>
         <v>10.921999999999999</v>
       </c>
       <c r="Q66">
-        <f>F66/6</f>
+        <f t="shared" si="29"/>
         <v>13.377333333333333</v>
       </c>
       <c r="R66">
-        <f>G66/6</f>
+        <f t="shared" si="29"/>
         <v>15.366999999999999</v>
       </c>
       <c r="S66">
-        <f>H66/6</f>
+        <f t="shared" si="29"/>
         <v>17.399000000000001</v>
       </c>
       <c r="T66">
-        <f>I66/6</f>
+        <f t="shared" si="29"/>
         <v>19.515666666666668</v>
       </c>
       <c r="U66">
-        <f>J66/6</f>
+        <f t="shared" si="29"/>
         <v>22.352</v>
       </c>
       <c r="V66">
-        <f>K66/6</f>
+        <f t="shared" si="29"/>
         <v>24.638000000000002</v>
       </c>
     </row>
@@ -4137,43 +4137,43 @@
         <v>165.86199999999999</v>
       </c>
       <c r="M67">
-        <f>B67/12</f>
+        <f t="shared" ref="M67:V67" si="30">B67/12</f>
         <v>3.0479999999999996</v>
       </c>
       <c r="N67">
-        <f>C67/12</f>
+        <f t="shared" si="30"/>
         <v>3.9158333333333335</v>
       </c>
       <c r="O67">
-        <f>D67/12</f>
+        <f t="shared" si="30"/>
         <v>5.1646666666666663</v>
       </c>
       <c r="P67">
-        <f>E67/12</f>
+        <f t="shared" si="30"/>
         <v>6.1595000000000004</v>
       </c>
       <c r="Q67">
-        <f>F67/12</f>
+        <f t="shared" si="30"/>
         <v>7.5564999999999998</v>
       </c>
       <c r="R67">
-        <f>G67/12</f>
+        <f t="shared" si="30"/>
         <v>8.6359999999999992</v>
       </c>
       <c r="S67">
-        <f>H67/12</f>
+        <f t="shared" si="30"/>
         <v>9.7789999999999999</v>
       </c>
       <c r="T67">
-        <f>I67/12</f>
+        <f t="shared" si="30"/>
         <v>10.943166666666665</v>
       </c>
       <c r="U67">
-        <f>J67/12</f>
+        <f t="shared" si="30"/>
         <v>12.573</v>
       </c>
       <c r="V67">
-        <f>K67/12</f>
+        <f t="shared" si="30"/>
         <v>13.821833333333332</v>
       </c>
     </row>
@@ -4212,43 +4212,43 @@
         <v>179.83199999999999</v>
       </c>
       <c r="M68">
-        <f>B68/24</f>
+        <f t="shared" ref="M68:V68" si="31">B68/24</f>
         <v>1.7145000000000001</v>
       </c>
       <c r="N68">
-        <f>C68/24</f>
+        <f t="shared" si="31"/>
         <v>2.2013333333333334</v>
       </c>
       <c r="O68">
-        <f>D68/24</f>
+        <f t="shared" si="31"/>
         <v>2.9104166666666664</v>
       </c>
       <c r="P68">
-        <f>E68/24</f>
+        <f t="shared" si="31"/>
         <v>3.4607499999999995</v>
       </c>
       <c r="Q68">
-        <f>F68/24</f>
+        <f t="shared" si="31"/>
         <v>4.2227500000000004</v>
       </c>
       <c r="R68">
-        <f>G68/24</f>
+        <f t="shared" si="31"/>
         <v>4.7942499999999999</v>
       </c>
       <c r="S68">
-        <f>H68/24</f>
+        <f t="shared" si="31"/>
         <v>5.3975</v>
       </c>
       <c r="T68">
-        <f>I68/24</f>
+        <f t="shared" si="31"/>
         <v>6.011333333333333</v>
       </c>
       <c r="U68">
-        <f>J68/24</f>
+        <f t="shared" si="31"/>
         <v>6.8474166666666667</v>
       </c>
       <c r="V68">
-        <f>K68/24</f>
+        <f t="shared" si="31"/>
         <v>7.4929999999999994</v>
       </c>
     </row>
@@ -4287,43 +4287,43 @@
         <v>218.18599999999998</v>
       </c>
       <c r="M69">
-        <f>B69/48</f>
+        <f t="shared" ref="M69:V69" si="32">B69/48</f>
         <v>0.9577916666666666</v>
       </c>
       <c r="N69">
-        <f>C69/48</f>
+        <f t="shared" si="32"/>
         <v>1.2329583333333332</v>
       </c>
       <c r="O69">
-        <f>D69/48</f>
+        <f t="shared" si="32"/>
         <v>1.6351249999999997</v>
       </c>
       <c r="P69">
-        <f>E69/48</f>
+        <f t="shared" si="32"/>
         <v>1.9632083333333332</v>
       </c>
       <c r="Q69">
-        <f>F69/48</f>
+        <f t="shared" si="32"/>
         <v>2.4182916666666667</v>
       </c>
       <c r="R69">
-        <f>G69/48</f>
+        <f t="shared" si="32"/>
         <v>2.7834166666666662</v>
       </c>
       <c r="S69">
-        <f>H69/48</f>
+        <f t="shared" si="32"/>
         <v>3.1644166666666664</v>
       </c>
       <c r="T69">
-        <f>I69/48</f>
+        <f t="shared" si="32"/>
         <v>3.5559999999999996</v>
       </c>
       <c r="U69">
-        <f>J69/48</f>
+        <f t="shared" si="32"/>
         <v>4.1063333333333327</v>
       </c>
       <c r="V69">
-        <f>K69/48</f>
+        <f t="shared" si="32"/>
         <v>4.5455416666666659</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed hella climate stuff
</commit_message>
<xml_diff>
--- a/climate/noaa_estimates.xlsx
+++ b/climate/noaa_estimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\MultiGrain\climate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5801DB1-300D-4D7E-A4F5-3B5A7953E9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32846E6-62BE-4054-8949-A3D4D0B878F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6168" yWindow="6468" windowWidth="7500" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All_Depth_English_PDS" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="40">
   <si>
     <t>Point precipitation frequency estimates (inches)</t>
   </si>
@@ -1008,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D28" workbookViewId="0">
-      <selection activeCell="R42" sqref="R42"/>
+    <sheetView tabSelected="1" topLeftCell="L37" workbookViewId="0">
+      <selection activeCell="V46" sqref="V46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1186,6 +1186,9 @@
       <c r="K15">
         <v>37.083999999999996</v>
       </c>
+      <c r="L15" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="M15">
         <f t="shared" ref="M15:V15" si="0">B15*12</f>
         <v>99.364800000000002</v>
@@ -1261,6 +1264,9 @@
       <c r="K16">
         <v>56.388000000000005</v>
       </c>
+      <c r="L16" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="M16">
         <f t="shared" ref="M16:V16" si="1">B16*6</f>
         <v>75.590400000000002</v>
@@ -1282,7 +1288,7 @@
         <v>188.976</v>
       </c>
       <c r="R16">
-        <f t="shared" si="1"/>
+        <f>G16*6</f>
         <v>214.88399999999996</v>
       </c>
       <c r="S16">
@@ -1336,6 +1342,9 @@
       <c r="K17">
         <v>69.849999999999994</v>
       </c>
+      <c r="L17" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="M17">
         <f t="shared" ref="M17:V17" si="2">B17*4</f>
         <v>62.483999999999995</v>
@@ -1411,6 +1420,9 @@
       <c r="K18">
         <v>94.233999999999995</v>
       </c>
+      <c r="L18" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="M18">
         <f t="shared" ref="M18:V18" si="3">B18*2</f>
         <v>42.062399999999997</v>
@@ -1486,6 +1498,9 @@
       <c r="K19">
         <v>116.58599999999998</v>
       </c>
+      <c r="L19" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="M19">
         <f t="shared" ref="M19:V19" si="4">B19</f>
         <v>26.161999999999999</v>
@@ -1561,6 +1576,9 @@
       <c r="K20">
         <v>147.57399999999998</v>
       </c>
+      <c r="L20" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="M20">
         <f t="shared" ref="M20:V20" si="5">B20/2</f>
         <v>14.731999999999998</v>
@@ -1636,6 +1654,9 @@
       <c r="K21">
         <v>159.00399999999999</v>
       </c>
+      <c r="L21" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="M21">
         <f t="shared" ref="M21:V21" si="6">B21/3</f>
         <v>10.583333333333334</v>
@@ -1711,6 +1732,9 @@
       <c r="K22">
         <v>176.78399999999999</v>
       </c>
+      <c r="L22" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="M22">
         <f t="shared" ref="M22:V22" si="7">B22/6</f>
         <v>6.0536666666666656</v>
@@ -1786,6 +1810,9 @@
       <c r="K23">
         <v>199.136</v>
       </c>
+      <c r="L23" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="M23">
         <f t="shared" ref="M23:V23" si="8">B23/12</f>
         <v>3.4713333333333325</v>
@@ -1861,6 +1888,9 @@
       <c r="K24">
         <v>213.10599999999999</v>
       </c>
+      <c r="L24" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="M24">
         <f t="shared" ref="M24:V24" si="9">B24/24</f>
         <v>1.9261666666666668</v>
@@ -1936,6 +1966,9 @@
       <c r="K25">
         <v>264.15999999999997</v>
       </c>
+      <c r="L25" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="M25">
         <f t="shared" ref="M25:V25" si="10">B25/48</f>
         <v>1.0900833333333333</v>
@@ -2011,6 +2044,9 @@
       <c r="K26">
         <v>284.47999999999996</v>
       </c>
+      <c r="L26" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -2046,6 +2082,9 @@
       <c r="K27">
         <v>307.33999999999997</v>
       </c>
+      <c r="L27" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -2081,6 +2120,9 @@
       <c r="K28">
         <v>353.06</v>
       </c>
+      <c r="L28" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -2116,6 +2158,9 @@
       <c r="K29">
         <v>398.78</v>
       </c>
+      <c r="L29" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -2151,6 +2196,9 @@
       <c r="K30">
         <v>449.58</v>
       </c>
+      <c r="L30" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -2186,6 +2234,9 @@
       <c r="K31">
         <v>497.84000000000003</v>
       </c>
+      <c r="L31" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -2361,6 +2412,9 @@
       <c r="K37">
         <v>42.417999999999999</v>
       </c>
+      <c r="L37" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="M37">
         <f t="shared" ref="M37:V37" si="11">B37*12</f>
         <v>113.99519999999998</v>
@@ -2436,6 +2490,9 @@
       <c r="K38">
         <v>64.515999999999991</v>
       </c>
+      <c r="L38" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="M38">
         <f t="shared" ref="M38:V38" si="12">B38*6</f>
         <v>86.867999999999995</v>
@@ -2511,6 +2568,9 @@
       <c r="K39">
         <v>79.756</v>
       </c>
+      <c r="L39" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="M39">
         <f t="shared" ref="M39:V39" si="13">B39*4</f>
         <v>71.729599999999991</v>
@@ -2586,6 +2646,9 @@
       <c r="K40">
         <v>107.696</v>
       </c>
+      <c r="L40" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="M40">
         <f t="shared" ref="M40:V40" si="14">B40*2</f>
         <v>48.26</v>
@@ -2661,6 +2724,9 @@
       <c r="K41">
         <v>133.096</v>
       </c>
+      <c r="L41" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="M41">
         <f t="shared" ref="M41:V41" si="15">B41</f>
         <v>29.971999999999998</v>
@@ -2736,6 +2802,9 @@
       <c r="K42">
         <v>167.13200000000001</v>
       </c>
+      <c r="L42" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="M42">
         <f t="shared" ref="M42:V42" si="16">B42/2</f>
         <v>16.890999999999998</v>
@@ -2811,6 +2880,9 @@
       <c r="K43">
         <v>179.578</v>
       </c>
+      <c r="L43" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="M43">
         <f t="shared" ref="M43:V43" si="17">B43/3</f>
         <v>12.107333333333331</v>
@@ -2886,6 +2958,9 @@
       <c r="K44">
         <v>198.88199999999998</v>
       </c>
+      <c r="L44" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="M44">
         <f t="shared" ref="M44:V44" si="18">B44/6</f>
         <v>6.9003333333333323</v>
@@ -2961,6 +3036,9 @@
       <c r="K45">
         <v>225.55200000000002</v>
       </c>
+      <c r="L45" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="M45">
         <f t="shared" ref="M45:V45" si="19">B45/12</f>
         <v>3.9581666666666666</v>
@@ -3036,6 +3114,9 @@
       <c r="K46">
         <v>240.792</v>
       </c>
+      <c r="L46" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="M46">
         <f t="shared" ref="M46:V46" si="20">B46/24</f>
         <v>2.1801666666666666</v>
@@ -3110,6 +3191,9 @@
       </c>
       <c r="K47">
         <v>302.26</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="M47">
         <f t="shared" ref="M47:V47" si="21">B47/48</f>

</xml_diff>